<commit_message>
Add: Web UI Test for Admin Page
</commit_message>
<xml_diff>
--- a/test_data/Stylish_TestCase.xlsx
+++ b/test_data/Stylish_TestCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Create Product Success"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="114">
   <si>
     <t>Receiver</t>
   </si>
@@ -359,6 +359,9 @@
   </si>
   <si>
     <t>S,M,L,XL,F</t>
+  </si>
+  <si>
+    <t>連身裙_Kathy</t>
   </si>
 </sst>
 </file>
@@ -408,13 +411,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Monospace"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Monospace"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -475,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -517,13 +520,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -540,10 +543,10 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="7" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -551,6 +554,12 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -876,11 +885,11 @@
     <col min="11" max="11" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="28" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -925,12 +934,12 @@
       </c>
       <c r="O1" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21.75">
       <c r="A2" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>58</v>
@@ -972,7 +981,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21.75">
       <c r="A3" s="1" t="s">
         <v>100</v>
       </c>
@@ -1017,7 +1026,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21.75">
       <c r="A4" s="1" t="s">
         <v>103</v>
       </c>
@@ -1057,7 +1066,7 @@
       <c r="M4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N4" s="26"/>
+      <c r="N4" s="27"/>
       <c r="O4" s="1" t="s">
         <v>107</v>
       </c>
@@ -1091,11 +1100,11 @@
     <col min="11" max="11" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="28" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -1140,7 +1149,7 @@
       </c>
       <c r="O1" s="26"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21.75">
       <c r="A2" s="1" t="s">
         <v>57</v>
       </c>
@@ -1187,7 +1196,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>68</v>
       </c>
@@ -1232,7 +1241,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
@@ -1272,7 +1281,7 @@
       <c r="M4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="N4" s="26"/>
+      <c r="N4" s="27"/>
       <c r="O4" s="1" t="s">
         <v>107</v>
       </c>
@@ -1289,14 +1298,14 @@
   </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="25" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
@@ -3593,7 +3602,7 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Add: API Test for Admin Product API
</commit_message>
<xml_diff>
--- a/test_data/Stylish_TestCase.xlsx
+++ b/test_data/Stylish_TestCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Create Product Success"/>
@@ -262,109 +262,112 @@
     <t>accessories</t>
   </si>
   <si>
+    <t>連衣裙_kathy</t>
+  </si>
+  <si>
+    <t>Description is required.</t>
+  </si>
+  <si>
+    <t>description cannot more than 255 characters.</t>
+  </si>
+  <si>
+    <t>Price is required.</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Price should be postive number.</t>
+  </si>
+  <si>
+    <t>Texture is required.</t>
+  </si>
+  <si>
+    <t>128 chars</t>
+  </si>
+  <si>
+    <t>texture cannot more than 127 characters.</t>
+  </si>
+  <si>
+    <t>Wash is required.</t>
+  </si>
+  <si>
+    <t>wash cannot more than 127 characters.</t>
+  </si>
+  <si>
+    <t>Place of Production is required.</t>
+  </si>
+  <si>
+    <t>place cannot more than 127 characters.</t>
+  </si>
+  <si>
+    <t>Note is required.</t>
+  </si>
+  <si>
+    <t>note cannot more than 127 characters.</t>
+  </si>
+  <si>
+    <t>Colors is required.</t>
+  </si>
+  <si>
+    <t>Sizes is required.</t>
+  </si>
+  <si>
+    <t>Story is required.</t>
+  </si>
+  <si>
+    <t>Main Image is required.</t>
+  </si>
+  <si>
+    <t>Other Images is required.</t>
+  </si>
+  <si>
+    <t>Category is required.</t>
+  </si>
+  <si>
+    <t>Category should be 'men', 'women' or 'accessories' Only</t>
+  </si>
+  <si>
+    <t>Color ID should be '1-7' Only</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Size should be 'S', 'M', 'L', 'XL', 'F' Only</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>白色</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>亮綠, 淺灰</t>
+  </si>
+  <si>
+    <t>L, XL</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
     <t>連衣裙</t>
   </si>
   <si>
-    <t>Description is required.</t>
-  </si>
-  <si>
-    <t>description cannot more than 255 characters.</t>
-  </si>
-  <si>
-    <t>Price is required.</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>Price should be postive number.</t>
-  </si>
-  <si>
-    <t>Texture is required.</t>
-  </si>
-  <si>
-    <t>128 chars</t>
-  </si>
-  <si>
-    <t>texture cannot more than 127 characters.</t>
-  </si>
-  <si>
-    <t>Wash is required.</t>
-  </si>
-  <si>
-    <t>wash cannot more than 127 characters.</t>
-  </si>
-  <si>
-    <t>Place of Production is required.</t>
-  </si>
-  <si>
-    <t>place cannot more than 127 characters.</t>
-  </si>
-  <si>
-    <t>Note is required.</t>
-  </si>
-  <si>
-    <t>note cannot more than 127 characters.</t>
-  </si>
-  <si>
-    <t>Colors is required.</t>
-  </si>
-  <si>
-    <t>Sizes is required.</t>
-  </si>
-  <si>
-    <t>Story is required.</t>
-  </si>
-  <si>
-    <t>Main Image is required.</t>
-  </si>
-  <si>
-    <t>Other Images is required.</t>
-  </si>
-  <si>
-    <t>Category is required.</t>
-  </si>
-  <si>
-    <t>Category should be 'men', 'women' or 'accessories' Only</t>
-  </si>
-  <si>
-    <t>Color ID should be '1-7' Only</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Size should be 'S', 'M', 'L', 'XL', 'F' Only</t>
-  </si>
-  <si>
-    <t>Colors</t>
-  </si>
-  <si>
-    <t>Women</t>
-  </si>
-  <si>
-    <t>白色</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Men</t>
-  </si>
-  <si>
-    <t>亮綠, 淺灰</t>
-  </si>
-  <si>
-    <t>L, XL</t>
-  </si>
-  <si>
-    <t>Accessories</t>
-  </si>
-  <si>
     <t>全選</t>
   </si>
   <si>
-    <t>連身裙</t>
+    <t>連身裙_Kathy</t>
   </si>
   <si>
     <t>棉質</t>
@@ -386,9 +389,6 @@
   </si>
   <si>
     <t>S,M,L,XL,F</t>
-  </si>
-  <si>
-    <t>連身裙_Kathy</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,6 +420,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Monospace"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -543,7 +549,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
@@ -561,13 +567,13 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -576,7 +582,7 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="7" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -585,7 +591,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -969,7 +975,7 @@
         <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>67</v>
@@ -978,7 +984,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>69</v>
@@ -1008,7 +1014,7 @@
         <v>75</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21.75">
@@ -1016,25 +1022,25 @@
         <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D3" s="22">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>110</v>
@@ -1043,7 +1049,7 @@
         <v>111</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>75</v>
@@ -1053,7 +1059,7 @@
         <v>75</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21.75">
@@ -1061,31 +1067,31 @@
         <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D4" s="22">
         <v>99999</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>74</v>
@@ -1098,7 +1104,7 @@
       </c>
       <c r="N4" s="28"/>
       <c r="O4" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1134,7 +1140,7 @@
     <col min="15" max="15" style="15" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -1184,7 +1190,7 @@
         <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>67</v>
@@ -1193,7 +1199,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>69</v>
@@ -1223,33 +1229,33 @@
         <v>75</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+        <v>117</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D3" s="22">
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>72</v>
@@ -1258,7 +1264,7 @@
         <v>73</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>75</v>
@@ -1268,7 +1274,7 @@
         <v>75</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
@@ -1276,31 +1282,31 @@
         <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D4" s="22">
         <v>99999</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>74</v>
@@ -1313,7 +1319,7 @@
       </c>
       <c r="N4" s="28"/>
       <c r="O4" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1493,7 +1499,7 @@
         <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="22">
@@ -1512,10 +1518,10 @@
         <v>71</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>74</v>
@@ -1538,7 +1544,7 @@
         <v>106</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>28</v>
@@ -1585,7 +1591,7 @@
         <v>106</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>67</v>
@@ -1630,7 +1636,7 @@
         <v>106</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>67</v>
@@ -1677,7 +1683,7 @@
         <v>106</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>67</v>
@@ -1724,7 +1730,7 @@
         <v>106</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>67</v>
@@ -1769,7 +1775,7 @@
         <v>106</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>67</v>
@@ -1816,7 +1822,7 @@
         <v>106</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>67</v>
@@ -1861,7 +1867,7 @@
         <v>106</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>67</v>
@@ -1908,7 +1914,7 @@
         <v>106</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>67</v>
@@ -1953,7 +1959,7 @@
         <v>106</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>67</v>
@@ -2000,7 +2006,7 @@
         <v>106</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>67</v>
@@ -2045,7 +2051,7 @@
         <v>106</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>67</v>
@@ -2092,7 +2098,7 @@
         <v>106</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>67</v>
@@ -2137,7 +2143,7 @@
         <v>106</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>67</v>
@@ -2182,7 +2188,7 @@
         <v>106</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>67</v>
@@ -2227,7 +2233,7 @@
         <v>106</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>67</v>
@@ -2272,7 +2278,7 @@
         <v>106</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>67</v>
@@ -2322,7 +2328,7 @@
   </sheetPr>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4165,7 +4171,7 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4175,9 +4181,9 @@
     <col min="4" max="4" style="15" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="15" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="17" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="15" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="17" width="8.719285714285713" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="17" width="6.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="15" width="5.147857142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="17" width="5.147857142857143" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="15" width="39.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -4200,13 +4206,13 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -4616,7 +4622,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="11"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="5"/>
       <c r="H16" s="12"/>
       <c r="I16" s="5">
         <v>1</v>

</xml_diff>